<commit_message>
Modified bill of material.
</commit_message>
<xml_diff>
--- a/Advance 3/Exercise 8/BOM - Alfredo Avila Gonzalez.xlsx
+++ b/Advance 3/Exercise 8/BOM - Alfredo Avila Gonzalez.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aavila/Dropbox/U/Sistemas Colaborativos I/Semana 8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5B789C1-980E-5746-84DB-8EF1FEADBC46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF75353-C457-CF43-BC74-4A5EC49F74A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{643D1BC4-DD45-0D4F-99FE-EB4411DDB912}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{643D1BC4-DD45-0D4F-99FE-EB4411DDB912}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Logical Platform" sheetId="1" r:id="rId1"/>
+    <sheet name="Logical Network Platform" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Component</t>
   </si>
@@ -112,13 +113,62 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>$0,10/h</t>
-  </si>
-  <si>
-    <t>$7632/h</t>
+    <t>Infrastructure Cost</t>
+  </si>
+  <si>
+    <t>$7.194/h</t>
+  </si>
+  <si>
+    <t>$0.10/h</t>
+  </si>
+  <si>
+    <t>Internet Gateway</t>
+  </si>
+  <si>
+    <t>CloudFront DNS</t>
+  </si>
+  <si>
+    <t>CloudFront WAF</t>
+  </si>
+  <si>
+    <t>API Gateway</t>
+  </si>
+  <si>
+    <t>Fully managed service that makes it easy for developers to create, publish, maintain, monitor, and secure APIs at any scale. APIs act as the "front door" for applications to access data, business logic, or functionality from your backend services. Using API Gateway, you can create RESTful APIs and WebSocket APIs that enable real-time two-way communication applications.</t>
+  </si>
+  <si>
+    <t>Web application firewall that helps protect your web applications or APIs against common web exploits that may affect availability, compromise security, or consume excessive resources.</t>
+  </si>
+  <si>
+    <t>Fast content delivery network (CDN) service that securely delivers data, videos, applications, and APIs to customers globally with low latency, high transfer speeds, all within a developer-friendly environment.</t>
+  </si>
+  <si>
+    <t>Horizontally scaled, redundant, and highly available VPC component that allows communication between your VPC and the internet.</t>
+  </si>
+  <si>
+    <t>#43243</t>
+  </si>
+  <si>
+    <t>#54354</t>
+  </si>
+  <si>
+    <t>#56456</t>
+  </si>
+  <si>
+    <t>#76765</t>
+  </si>
+  <si>
+    <t>$1/300M</t>
+  </si>
+  <si>
+    <t>$6+-/h + 
+$0.6/1M Req</t>
+  </si>
+  <si>
+    <t>$0.4/1M</t>
+  </si>
+  <si>
+    <t>$0.015/h per ENI</t>
   </si>
 </sst>
 </file>
@@ -510,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DFF416-1122-1D45-9572-B110523A1F0C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="199" zoomScaleNormal="199" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="199" zoomScaleNormal="199" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,7 +573,8 @@
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -592,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -638,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -686,14 +737,143 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372BEF80-933B-7B45-B36A-A717BFBD411A}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>